<commit_message>
Log in method has been changed and DataProvider has been added into TestBase
</commit_message>
<xml_diff>
--- a/src/test/resources/Vytracktestdata.xlsx
+++ b/src/test/resources/Vytracktestdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="11760" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="QA1-all" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3847" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3841" uniqueCount="1475">
   <si>
     <t>username</t>
   </si>
@@ -4799,7 +4799,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9053,7 +9053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -18343,10 +18343,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -18357,33 +18357,9 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" t="s">
         <v>1472</v>
       </c>
     </row>

</xml_diff>